<commit_message>
Updated translated and final datasets with change in records
</commit_message>
<xml_diff>
--- a/records/Hrudai_records_translation.xlsx
+++ b/records/Hrudai_records_translation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="174">
   <si>
     <t>Category</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve"> Opening the batting and bowling in the same match </t>
   </si>
   <si>
-    <t>ఒకేే మ్యాచ్ లో జట్టు బ్యాటింగ్, బౌలింగ్ ను handle_gender_3</t>
+    <t>ఒకేే మ్యాచ్ లో జట్టుకు బ్యాటింగ్, బౌలింగ్ ను handle_gender_3</t>
   </si>
   <si>
     <t xml:space="preserve">handle_gender_2 = సాధించాడు / సాధించింది </t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve"> 1000 runs, 50 wickets and 50 catches </t>
   </si>
   <si>
-    <t xml:space="preserve"> 50 క్యాచ్లు , 50 వికెట్లు, 1000 పరుగులు handle_gender</t>
+    <t>1000 పరుగులు, 50 వికెట్లు, 50 క్యాచ్లు  handle_gender</t>
   </si>
   <si>
     <t xml:space="preserve"> Representing two countries </t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve"> Hundred and a ninety in a match </t>
   </si>
   <si>
-    <t xml:space="preserve"> ఒకే మ్యాచ్ లో శతకం, తొంభై పరుగులు handle_gender</t>
+    <t xml:space="preserve"> ఒకే టెస్ట్ మ్యాచ్ లో శతకం, తొంభై పరుగులు handle_gender</t>
   </si>
   <si>
     <t xml:space="preserve"> 99 not out (and 199, 299 etc) (99*)</t>
@@ -223,19 +223,19 @@
     <t xml:space="preserve"> Unusual dismissals (handled the bal)</t>
   </si>
   <si>
-    <t>కెరీర్ లో ఒక సరి బాల్ ని హాండిల్ చేసి అవుట్ అయిన ఆటగాళ్ల</t>
+    <t>కెరీర్ లో బాల్ ని హాండిల్ చేసి అవుట్ అయిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Unusual dismissals (retired out)</t>
   </si>
   <si>
-    <t>కెరీర్ లో ఒకసారి రిటైర్డ్ హర్ట్ అవ్వడం వల్ల అవుట్ అయిన ఆటగాళ్ల</t>
+    <t>కెరీర్ లో రిటైర్డ్ హర్ట్ అవ్వడం వల్ల అవుట్ అయిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Unusual dismissals (obstructing the)</t>
   </si>
   <si>
-    <t>కెరీర్ లో ఒకసారి ఫీల్డ్ ని ఒబ్ష్ట్రక్ట్  చేయడం వల్ల అవుట్ అయిన ఆటగాళ్ల</t>
+    <t>కెరీర్ లో ఫీల్డ్ ని అడ్డుకోవడం వల్ల అవుట్ అయిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t>Only statistic</t>
@@ -250,7 +250,7 @@
     <t xml:space="preserve"> Carrying bat through a completed innings </t>
   </si>
   <si>
-    <t>ఒక మ్యాచ్ లో ఓపెనింగ్ బాట్స్మన్ గా వచ్చి ఇన్నింగ్స్ చివరి వరకు నాట్ అవుట్ గా handle_gender_5</t>
+    <t>ఒక మ్యాచ్ లో ఓపెనర్ గా వచ్చి ఇన్నింగ్స్ చివరి వరకు నాట్ అవుట్ గా handle_gender_5</t>
   </si>
   <si>
     <t>Both rank and statistic present</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve"> Captains who have kept wicket and opened the batting </t>
   </si>
   <si>
-    <t xml:space="preserve"> వికెట్ కీపింగ్ చేసి జట్టుకు బ్యాటింగ్ ప్రారంభించిన కెప్టెన్ళ్</t>
+    <t>కెప్టెన్ గా వికెట్ కీపింగ్, బ్యాటింగ్ ప్రారంభించిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Most matches as a match referee </t>
@@ -271,13 +271,13 @@
     <t xml:space="preserve"> Highest partnership for the fifth wicket </t>
   </si>
   <si>
-    <t xml:space="preserve"> ఐదో వికెట్ కు అత్యధిక భాగస్వామ్యంగ ఉన్న ఆటగాళ్ల</t>
+    <t xml:space="preserve"> ఐదో వికెట్ కు అత్యధిక భాగస్వామ్యంగా ఉన్న ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Oldest player to take a maiden five-wickets-in-an-innings </t>
   </si>
   <si>
-    <t xml:space="preserve"> ఒకే ఇన్నింగ్స్ లో మొదటి సారి ఐదు వికెట్లు సాధించిన వయసయిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> ఒకే ఇన్నింగ్స్ లో మొదటి సారి ఐదు వికెట్లు సాధించిన పురాతన ( ఓల్డ్ ) ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Most hundreds in a series </t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve"> Oldest player to take ten-wickets-in-a-match </t>
   </si>
   <si>
-    <t xml:space="preserve"> ఒకే మ్యాచ్ లో పది వికెట్లు సాధించిన వయసయిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> ఒకే మ్యాచ్ లో పది వికెట్లు సాధించిన పురాతన ( ఓల్డ్ ) ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Most catches in career </t>
@@ -337,7 +337,7 @@
     <t xml:space="preserve"> Oldest players </t>
   </si>
   <si>
-    <t>వయసయిన ఆటగాళ్ల</t>
+    <t>పురాతన ( ఓల్డ్ ) ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Hundreds in consecutive matches from debut </t>
@@ -361,7 +361,7 @@
     <t xml:space="preserve"> Most wickets taken caught by a fielder </t>
   </si>
   <si>
-    <t>ఫీల్డర్ క్యాచ్ చేసి అత్యధిక వికెట్లు సాధించిన ఆటగాళ్ల</t>
+    <t>ఫీల్డర్ క్యాచ్ పట్టడం ద్వారా అత్యధిక వికెట్లు సాధించిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Best figures in a match when on the losing side </t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve"> Most runs in an innings by a captain </t>
   </si>
   <si>
-    <t xml:space="preserve"> కెప్టెన్ గ ఒకే ఇన్నింగ్స్ లో అత్యధిక పరుగులు చేసిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> కెప్టెన్ గా ఒకే ఇన్నింగ్స్ లో అత్యధిక పరుగులు చేసిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Highest partnership for the fourth wicket </t>
@@ -397,7 +397,7 @@
     <t xml:space="preserve"> Most pairs in career </t>
   </si>
   <si>
-    <t xml:space="preserve"> కెరీర్ లో అత్యధిక మ్యాచ్‌లలో రెండు ఇన్నింగ్సలలో డక్ అవుట్ అయిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> కెరీర్ లో అత్యధిక మ్యాచ్‌లలో రెండు ఇన్నింగ్స్ లలో డక్ అవుట్ అయిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Hundreds in consecutive innings </t>
@@ -421,7 +421,7 @@
     <t xml:space="preserve"> No ducks in career </t>
   </si>
   <si>
-    <t>కెరీర్ లో డక్ అవుట్ అవ్వని ఆటగాళ్ల</t>
+    <t>కెరీర్ లో ఒక్కసారి కూడా డక్ అవుట్ అవ్వని ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Highest percentage of runs in a completed innings </t>
@@ -457,19 +457,19 @@
     <t xml:space="preserve"> Oldest captains </t>
   </si>
   <si>
-    <t xml:space="preserve"> వయసయిన కెప్టెన్ల</t>
+    <t xml:space="preserve"> పురాతన ( ఓల్డ్ ) కెప్టెన్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Highest partnerships for any wicket </t>
   </si>
   <si>
-    <t xml:space="preserve"> ఏ వికెట్ కైనా అత్యధిక భాగస్వామ్యామ్యం వహించిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> ఏ వికెట్ కైనా అత్యధిక భాగస్వామ్యం వహించిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Most runs in an innings by a wicketkeeper </t>
   </si>
   <si>
-    <t xml:space="preserve"> వికెట్ కీపర్ గ ఉన్న ఇన్నింగ్స్ లో అత్యధిక పరుగులు చేసిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> వికెట్ కీపర్ గా ఒక ఇన్నింగ్స్ లో అత్యధిక పరుగులు చేసిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Worst career economy rate </t>
@@ -487,7 +487,7 @@
     <t xml:space="preserve"> Fifties in consecutive matches </t>
   </si>
   <si>
-    <t xml:space="preserve"> వరుస మ్యాచ్ లలో అర్ధ శతకం చేసిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> వరుస మ్యాచ్ లలో అర్ధ శతకాలు చేసిన ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Bowler/batters combinations </t>
@@ -517,7 +517,7 @@
     <t xml:space="preserve"> Oldest player to take five-wickets-in-an-innings </t>
   </si>
   <si>
-    <t xml:space="preserve"> ఒకే ఇన్నింగ్స్ లో ఐదు వికెట్లు  సాధించిన వయసయిన ఆటగాళ్ల</t>
+    <t xml:space="preserve"> ఒకే ఇన్నింగ్స్ లో ఐదు వికెట్లు  సాధించిన పురాతన ( ఓల్డ్ ) ఆటగాళ్ల</t>
   </si>
   <si>
     <t xml:space="preserve"> Fastest to 10000 runs </t>
@@ -530,13 +530,16 @@
   </si>
   <si>
     <t>సిరీస్ లో అత్యధిక డబుల్ సెంచరీలు చేసిన ఆటగాళ్ల</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -551,11 +554,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF202124"/>
       <name val="Inherit"/>
+    </font>
+    <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -608,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -616,19 +624,22 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -877,7 +888,7 @@
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -891,7 +902,7 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -908,10 +919,10 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -962,7 +973,7 @@
       <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -976,7 +987,7 @@
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1172,7 +1183,7 @@
       <c r="C22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1186,7 +1197,7 @@
       <c r="C23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1200,7 +1211,7 @@
       <c r="C24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1298,7 +1309,7 @@
       <c r="C31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1312,7 +1323,7 @@
       <c r="C32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1326,7 +1337,7 @@
       <c r="C33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1354,7 +1365,7 @@
       <c r="C35" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1368,7 +1379,7 @@
       <c r="C36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="6" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1396,7 +1407,7 @@
       <c r="C38" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1410,7 +1421,7 @@
       <c r="C39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="5" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1424,7 +1435,7 @@
       <c r="C40" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="5" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1480,7 +1491,7 @@
       <c r="C44" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1550,7 +1561,7 @@
       <c r="C49" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="5" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1564,7 +1575,7 @@
       <c r="C50" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1606,7 +1617,7 @@
       <c r="C53" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="4" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1634,7 +1645,7 @@
       <c r="C55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="5" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1690,7 +1701,7 @@
       <c r="C59" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1718,7 +1729,7 @@
       <c r="C61" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="8" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1746,7 +1757,7 @@
       <c r="C63" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="5" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1788,7 +1799,7 @@
       <c r="C66" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="8" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1816,7 +1827,7 @@
       <c r="C68" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="8" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1830,7 +1841,7 @@
       <c r="C69" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="5" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1844,7 +1855,7 @@
       <c r="C70" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="5" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1858,7 +1869,7 @@
       <c r="C71" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="5" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1900,7 +1911,7 @@
       <c r="C74" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" s="5" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1914,7 +1925,7 @@
       <c r="C75" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="3" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1970,7 +1981,7 @@
       <c r="C79" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" s="5" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1984,7 +1995,7 @@
       <c r="C80" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2022,7 +2033,11 @@
     <row r="99" ht="15.75" customHeight="1"/>
     <row r="100" ht="15.75" customHeight="1"/>
     <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1">
+      <c r="C102" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
     <row r="103" ht="15.75" customHeight="1"/>
     <row r="104" ht="15.75" customHeight="1"/>
     <row r="105" ht="15.75" customHeight="1"/>

</xml_diff>